<commit_message>
Sets ELC-technology availabillity for the new regions
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_ELC_Techs_Trans.xlsx
+++ b/SubRES_TMPL/SubRes_ELC_Techs_Trans.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2bae57ad8ea7bb4f/OneDrive/GitHub^J Inc/EnergyIsland/SubRES_TMPL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{DD7FDB20-4823-44BF-BD66-560DB5130607}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E3A8498-6025-45DA-9945-D62F66141049}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="13_ncr:1_{DD7FDB20-4823-44BF-BD66-560DB5130607}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C1809353-6B38-4C64-AD5C-9FADB893F2A8}"/>
   <bookViews>
-    <workbookView xWindow="3218" yWindow="3218" windowWidth="16875" windowHeight="10522" tabRatio="733" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3000" yWindow="915" windowWidth="16875" windowHeight="10523" tabRatio="733" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LOG" sheetId="11" r:id="rId1"/>
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="44">
   <si>
     <t>Year</t>
   </si>
@@ -217,19 +217,7 @@
     <t>ERWINELCWIN5N</t>
   </si>
   <si>
-    <t>SUPH2ALKC1N</t>
-  </si>
-  <si>
-    <t>SUPH2ALKC2N</t>
-  </si>
-  <si>
-    <t>SUPH2PEMC1N</t>
-  </si>
-  <si>
-    <t>SUPH2PEMC2N</t>
-  </si>
-  <si>
-    <t>SUPH2SOEC2N</t>
+    <t>*</t>
   </si>
 </sst>
 </file>
@@ -25824,7 +25812,7 @@
   </sheetPr>
   <dimension ref="B4:J39"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="81" workbookViewId="0">
+    <sheetView zoomScale="81" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -26405,8 +26393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8EF56F5-FFEC-4195-B835-F2DA1F364DE3}">
   <dimension ref="B3:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25"/>
@@ -26450,37 +26438,40 @@
       </c>
     </row>
     <row r="5" spans="2:10">
-      <c r="F5">
+      <c r="C5">
         <v>1</v>
       </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
       <c r="G5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="2:10">
-      <c r="F6" s="11">
+      <c r="F6">
         <v>1</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6">
         <v>1</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6">
         <v>1</v>
       </c>
-      <c r="I6" s="11">
+      <c r="I6">
         <v>1</v>
       </c>
-      <c r="J6" s="11" t="s">
-        <v>42</v>
+      <c r="J6" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="2:10">
@@ -26496,77 +26487,37 @@
       <c r="I7" s="11">
         <v>1</v>
       </c>
-      <c r="J7" s="42" t="s">
-        <v>43</v>
+      <c r="J7" s="11" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="2:10">
-      <c r="F8" s="11">
-        <v>1</v>
-      </c>
-      <c r="G8" s="11">
-        <v>1</v>
-      </c>
-      <c r="H8" s="11">
-        <v>1</v>
-      </c>
-      <c r="I8" s="11">
-        <v>1</v>
-      </c>
-      <c r="J8" s="42" t="s">
-        <v>44</v>
-      </c>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="42"/>
     </row>
     <row r="9" spans="2:10">
-      <c r="F9" s="11">
-        <v>1</v>
-      </c>
-      <c r="G9" s="11">
-        <v>1</v>
-      </c>
-      <c r="H9" s="11">
-        <v>1</v>
-      </c>
-      <c r="I9" s="11">
-        <v>1</v>
-      </c>
-      <c r="J9" s="42" t="s">
-        <v>45</v>
-      </c>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="42"/>
     </row>
     <row r="10" spans="2:10">
-      <c r="F10" s="11">
-        <v>1</v>
-      </c>
-      <c r="G10" s="11">
-        <v>1</v>
-      </c>
-      <c r="H10" s="11">
-        <v>1</v>
-      </c>
-      <c r="I10" s="11">
-        <v>1</v>
-      </c>
-      <c r="J10" s="42" t="s">
-        <v>46</v>
-      </c>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="42"/>
     </row>
     <row r="11" spans="2:10">
-      <c r="F11" s="11">
-        <v>1</v>
-      </c>
-      <c r="G11" s="11">
-        <v>1</v>
-      </c>
-      <c r="H11" s="11">
-        <v>1</v>
-      </c>
-      <c r="I11" s="11">
-        <v>1</v>
-      </c>
-      <c r="J11" s="42" t="s">
-        <v>47</v>
-      </c>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="42"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix name elc ava
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_ELC_Techs_Trans.xlsx
+++ b/SubRES_TMPL/SubRes_ELC_Techs_Trans.xlsx
@@ -5,17 +5,17 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2bae57ad8ea7bb4f/OneDrive/GitHub^J Inc/EnergyIsland/SubRES_TMPL/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES Modeller\TIMES-TOM\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="13_ncr:1_{DD7FDB20-4823-44BF-BD66-560DB5130607}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C1809353-6B38-4C64-AD5C-9FADB893F2A8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46B5BE3A-A333-4CEC-81A9-DC957746DCE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="915" windowWidth="16875" windowHeight="10523" tabRatio="733" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="733" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LOG" sheetId="11" r:id="rId1"/>
     <sheet name="ELC_Constraint" sheetId="12" r:id="rId2"/>
-    <sheet name="Availability" sheetId="13" r:id="rId3"/>
+    <sheet name="ELC_AVA" sheetId="13" r:id="rId3"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId4"/>
@@ -6056,7 +6056,6 @@
     <cellStyle name="Bad 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
     <cellStyle name="Bad 3" xfId="2012" xr:uid="{00000000-0005-0000-0000-000045000000}"/>
     <cellStyle name="Bad 4" xfId="3310" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="4489" builtinId="9" hidden="1"/>
     <cellStyle name="Bruger data" xfId="661" xr:uid="{00000000-0005-0000-0000-000047000000}"/>
     <cellStyle name="Calcolo" xfId="31" xr:uid="{00000000-0005-0000-0000-000048000000}"/>
     <cellStyle name="Calcolo 2" xfId="3311" xr:uid="{00000000-0005-0000-0000-000049000000}"/>
@@ -6751,7 +6750,9 @@
     <cellStyle name="Euro 9 4 3" xfId="2312" xr:uid="{00000000-0005-0000-0000-0000FA020000}"/>
     <cellStyle name="Euro 9 5" xfId="953" xr:uid="{00000000-0005-0000-0000-0000FB020000}"/>
     <cellStyle name="Fixed2 - Type2" xfId="7" xr:uid="{00000000-0005-0000-0000-0000FC020000}"/>
+    <cellStyle name="Followed Hyperlink" xfId="4489" builtinId="9" hidden="1"/>
     <cellStyle name="Good 2" xfId="3372" xr:uid="{00000000-0005-0000-0000-0000FE020000}"/>
+    <cellStyle name="Hyperlink" xfId="4488" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink 2" xfId="954" xr:uid="{00000000-0005-0000-0000-000000030000}"/>
     <cellStyle name="Hyperlink 2 2" xfId="3373" xr:uid="{00000000-0005-0000-0000-000001030000}"/>
     <cellStyle name="Input 2" xfId="84" xr:uid="{00000000-0005-0000-0000-000002030000}"/>
@@ -6774,7 +6775,6 @@
     <cellStyle name="Komma 5" xfId="962" xr:uid="{00000000-0005-0000-0000-000013030000}"/>
     <cellStyle name="Komma 5 2" xfId="2315" xr:uid="{00000000-0005-0000-0000-000014030000}"/>
     <cellStyle name="Kontroller celle" xfId="3380" xr:uid="{00000000-0005-0000-0000-000015030000}"/>
-    <cellStyle name="Link" xfId="4488" builtinId="8" hidden="1"/>
     <cellStyle name="Link 2" xfId="963" xr:uid="{00000000-0005-0000-0000-000016030000}"/>
     <cellStyle name="Link 3" xfId="964" xr:uid="{00000000-0005-0000-0000-000017030000}"/>
     <cellStyle name="Markeringsfarve1" xfId="3381" xr:uid="{00000000-0005-0000-0000-000018030000}"/>
@@ -8463,6 +8463,7 @@
     <cellStyle name="Neutral 2" xfId="441" xr:uid="{00000000-0005-0000-0000-0000AB090000}"/>
     <cellStyle name="Neutral 2 2" xfId="4165" xr:uid="{00000000-0005-0000-0000-0000AC090000}"/>
     <cellStyle name="Neutrale" xfId="206" xr:uid="{00000000-0005-0000-0000-0000AD090000}"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 10" xfId="1325" xr:uid="{00000000-0005-0000-0000-0000AF090000}"/>
     <cellStyle name="Normal 10 2" xfId="2615" xr:uid="{00000000-0005-0000-0000-0000B0090000}"/>
     <cellStyle name="Normal 10 2 2" xfId="4492" xr:uid="{5BB6BF09-EA62-41EC-8DE0-DAD0CC0557AE}"/>
@@ -10403,7 +10404,6 @@
     <cellStyle name="Procent 3 3" xfId="4425" xr:uid="{00000000-0005-0000-0000-00003E110000}"/>
     <cellStyle name="Procent 4" xfId="2005" xr:uid="{00000000-0005-0000-0000-00003F110000}"/>
     <cellStyle name="Procent 4 2" xfId="3264" xr:uid="{00000000-0005-0000-0000-000040110000}"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Style 155" xfId="4426" xr:uid="{00000000-0005-0000-0000-000042110000}"/>
     <cellStyle name="Style 156" xfId="4427" xr:uid="{00000000-0005-0000-0000-000043110000}"/>
     <cellStyle name="Style 157" xfId="4428" xr:uid="{00000000-0005-0000-0000-000044110000}"/>
@@ -25175,13 +25175,13 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="7.46484375" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="7.453125" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="11.46484375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="18.46484375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="172.86328125" customWidth="1"/>
-    <col min="6" max="6" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="172.81640625" customWidth="1"/>
+    <col min="6" max="6" width="23.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:6">
@@ -25769,34 +25769,34 @@
       <c r="D66" s="4"/>
       <c r="E66" s="4"/>
     </row>
-    <row r="71" spans="1:5" ht="15.4">
+    <row r="71" spans="1:5" ht="15.5">
       <c r="D71" s="3"/>
     </row>
-    <row r="72" spans="1:5" ht="15.4">
+    <row r="72" spans="1:5" ht="15.5">
       <c r="D72" s="3"/>
     </row>
-    <row r="73" spans="1:5" ht="15.4">
+    <row r="73" spans="1:5" ht="15.5">
       <c r="D73" s="3"/>
     </row>
-    <row r="74" spans="1:5" ht="15.4">
+    <row r="74" spans="1:5" ht="15.5">
       <c r="D74" s="3"/>
     </row>
-    <row r="75" spans="1:5" ht="15.4">
+    <row r="75" spans="1:5" ht="15.5">
       <c r="D75" s="3"/>
     </row>
-    <row r="76" spans="1:5" ht="15.4">
+    <row r="76" spans="1:5" ht="15.5">
       <c r="D76" s="3"/>
     </row>
-    <row r="77" spans="1:5" ht="15.4">
+    <row r="77" spans="1:5" ht="15.5">
       <c r="D77" s="3"/>
     </row>
-    <row r="78" spans="1:5" ht="15.4">
+    <row r="78" spans="1:5" ht="15.5">
       <c r="D78" s="3"/>
     </row>
-    <row r="79" spans="1:5" ht="15.4">
+    <row r="79" spans="1:5" ht="15.5">
       <c r="D79" s="3"/>
     </row>
-    <row r="80" spans="1:5" ht="15.4">
+    <row r="80" spans="1:5" ht="15.5">
       <c r="D80" s="3"/>
     </row>
   </sheetData>
@@ -25816,11 +25816,11 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="7.46484375" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="7.453125" defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="3" width="17.86328125" customWidth="1"/>
-    <col min="4" max="4" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="9" width="17.86328125" customWidth="1"/>
+    <col min="2" max="3" width="17.81640625" customWidth="1"/>
+    <col min="4" max="4" width="29.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="9" width="17.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:9">
@@ -25835,7 +25835,7 @@
       <c r="H4" s="20"/>
       <c r="I4" s="21"/>
     </row>
-    <row r="5" spans="2:9" ht="14.65" thickBot="1">
+    <row r="5" spans="2:9" ht="15" thickBot="1">
       <c r="B5" s="22" t="s">
         <v>12</v>
       </c>
@@ -26208,7 +26208,7 @@
       </c>
       <c r="I28" s="26"/>
     </row>
-    <row r="29" spans="2:10" ht="28.5">
+    <row r="29" spans="2:10" ht="29">
       <c r="B29" s="26"/>
       <c r="C29" s="33" t="s">
         <v>22</v>
@@ -26220,7 +26220,7 @@
       <c r="H29" s="33"/>
       <c r="I29" s="26"/>
     </row>
-    <row r="30" spans="2:10" ht="14.65" thickBot="1">
+    <row r="30" spans="2:10" ht="15" thickBot="1">
       <c r="B30" s="26"/>
       <c r="C30" s="34" t="s">
         <v>23</v>
@@ -26394,10 +26394,10 @@
   <dimension ref="B3:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="3" spans="2:10">
       <c r="B3" s="37" t="s">
@@ -26408,7 +26408,7 @@
       <c r="E3" s="38"/>
       <c r="F3" s="11"/>
     </row>
-    <row r="4" spans="2:10" ht="14.65" thickBot="1">
+    <row r="4" spans="2:10" ht="15" thickBot="1">
       <c r="B4" s="39" t="s">
         <v>12</v>
       </c>
@@ -26438,7 +26438,10 @@
       </c>
     </row>
     <row r="5" spans="2:10">
-      <c r="C5">
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
         <v>1</v>
       </c>
       <c r="F5">
@@ -26458,6 +26461,12 @@
       </c>
     </row>
     <row r="6" spans="2:10">
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
       <c r="F6">
         <v>1</v>
       </c>
@@ -26475,6 +26484,12 @@
       </c>
     </row>
     <row r="7" spans="2:10">
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
       <c r="F7" s="11">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Update name in trans file
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_ELC_Techs_Trans.xlsx
+++ b/SubRES_TMPL/SubRes_ELC_Techs_Trans.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES Modeller\TIMES-TOM\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46B5BE3A-A333-4CEC-81A9-DC957746DCE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CCC5AF4-F69C-49E8-992F-C890BE885661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="733" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -199,9 +199,6 @@
     <t>AllRegions</t>
   </si>
   <si>
-    <t>DHISLBH</t>
-  </si>
-  <si>
     <t>DKISL1</t>
   </si>
   <si>
@@ -218,6 +215,9 @@
   </si>
   <si>
     <t>*</t>
+  </si>
+  <si>
+    <t>DKISLBH</t>
   </si>
 </sst>
 </file>
@@ -26394,7 +26394,7 @@
   <dimension ref="B3:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5"/>
@@ -26422,16 +26422,16 @@
         <v>34</v>
       </c>
       <c r="F4" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="G4" s="40" t="s">
+      <c r="H4" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="H4" s="40" t="s">
+      <c r="I4" s="40" t="s">
         <v>39</v>
-      </c>
-      <c r="I4" s="40" t="s">
-        <v>40</v>
       </c>
       <c r="J4" s="41" t="s">
         <v>15</v>
@@ -26457,7 +26457,7 @@
         <v>0</v>
       </c>
       <c r="J5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="2:10">
@@ -26480,7 +26480,7 @@
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="2:10">
@@ -26503,7 +26503,7 @@
         <v>1</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="2:10">

</xml_diff>

<commit_message>
Only make PV available in MAR
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_ELC_Techs_Trans.xlsx
+++ b/SubRES_TMPL/SubRes_ELC_Techs_Trans.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES Modeller\TIMES-TOM\SubRES_TMPL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2bae57ad8ea7bb4f/OneDrive/GitHub^J Inc/EnergyIsland/SubRES_TMPL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CCC5AF4-F69C-49E8-992F-C890BE885661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{3CCC5AF4-F69C-49E8-992F-C890BE885661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2D61B342-B128-4C57-95D3-F79313A6E228}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="733" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="44880" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="733" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LOG" sheetId="11" r:id="rId1"/>
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="46">
   <si>
     <t>Year</t>
   </si>
@@ -218,6 +218,12 @@
   </si>
   <si>
     <t>DKISLBH</t>
+  </si>
+  <si>
+    <t>MAR</t>
+  </si>
+  <si>
+    <t>ERSOLPV5N</t>
   </si>
 </sst>
 </file>
@@ -6056,6 +6062,7 @@
     <cellStyle name="Bad 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
     <cellStyle name="Bad 3" xfId="2012" xr:uid="{00000000-0005-0000-0000-000045000000}"/>
     <cellStyle name="Bad 4" xfId="3310" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="4489" builtinId="9" hidden="1"/>
     <cellStyle name="Bruger data" xfId="661" xr:uid="{00000000-0005-0000-0000-000047000000}"/>
     <cellStyle name="Calcolo" xfId="31" xr:uid="{00000000-0005-0000-0000-000048000000}"/>
     <cellStyle name="Calcolo 2" xfId="3311" xr:uid="{00000000-0005-0000-0000-000049000000}"/>
@@ -6750,9 +6757,7 @@
     <cellStyle name="Euro 9 4 3" xfId="2312" xr:uid="{00000000-0005-0000-0000-0000FA020000}"/>
     <cellStyle name="Euro 9 5" xfId="953" xr:uid="{00000000-0005-0000-0000-0000FB020000}"/>
     <cellStyle name="Fixed2 - Type2" xfId="7" xr:uid="{00000000-0005-0000-0000-0000FC020000}"/>
-    <cellStyle name="Followed Hyperlink" xfId="4489" builtinId="9" hidden="1"/>
     <cellStyle name="Good 2" xfId="3372" xr:uid="{00000000-0005-0000-0000-0000FE020000}"/>
-    <cellStyle name="Hyperlink" xfId="4488" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink 2" xfId="954" xr:uid="{00000000-0005-0000-0000-000000030000}"/>
     <cellStyle name="Hyperlink 2 2" xfId="3373" xr:uid="{00000000-0005-0000-0000-000001030000}"/>
     <cellStyle name="Input 2" xfId="84" xr:uid="{00000000-0005-0000-0000-000002030000}"/>
@@ -6775,6 +6780,7 @@
     <cellStyle name="Komma 5" xfId="962" xr:uid="{00000000-0005-0000-0000-000013030000}"/>
     <cellStyle name="Komma 5 2" xfId="2315" xr:uid="{00000000-0005-0000-0000-000014030000}"/>
     <cellStyle name="Kontroller celle" xfId="3380" xr:uid="{00000000-0005-0000-0000-000015030000}"/>
+    <cellStyle name="Link" xfId="4488" builtinId="8" hidden="1"/>
     <cellStyle name="Link 2" xfId="963" xr:uid="{00000000-0005-0000-0000-000016030000}"/>
     <cellStyle name="Link 3" xfId="964" xr:uid="{00000000-0005-0000-0000-000017030000}"/>
     <cellStyle name="Markeringsfarve1" xfId="3381" xr:uid="{00000000-0005-0000-0000-000018030000}"/>
@@ -8463,7 +8469,6 @@
     <cellStyle name="Neutral 2" xfId="441" xr:uid="{00000000-0005-0000-0000-0000AB090000}"/>
     <cellStyle name="Neutral 2 2" xfId="4165" xr:uid="{00000000-0005-0000-0000-0000AC090000}"/>
     <cellStyle name="Neutrale" xfId="206" xr:uid="{00000000-0005-0000-0000-0000AD090000}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 10" xfId="1325" xr:uid="{00000000-0005-0000-0000-0000AF090000}"/>
     <cellStyle name="Normal 10 2" xfId="2615" xr:uid="{00000000-0005-0000-0000-0000B0090000}"/>
     <cellStyle name="Normal 10 2 2" xfId="4492" xr:uid="{5BB6BF09-EA62-41EC-8DE0-DAD0CC0557AE}"/>
@@ -10404,6 +10409,7 @@
     <cellStyle name="Procent 3 3" xfId="4425" xr:uid="{00000000-0005-0000-0000-00003E110000}"/>
     <cellStyle name="Procent 4" xfId="2005" xr:uid="{00000000-0005-0000-0000-00003F110000}"/>
     <cellStyle name="Procent 4 2" xfId="3264" xr:uid="{00000000-0005-0000-0000-000040110000}"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Style 155" xfId="4426" xr:uid="{00000000-0005-0000-0000-000042110000}"/>
     <cellStyle name="Style 156" xfId="4427" xr:uid="{00000000-0005-0000-0000-000043110000}"/>
     <cellStyle name="Style 157" xfId="4428" xr:uid="{00000000-0005-0000-0000-000044110000}"/>
@@ -25175,13 +25181,13 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.453125" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="7.46484375" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="172.81640625" customWidth="1"/>
-    <col min="6" max="6" width="23.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.46484375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="18.46484375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="172.796875" customWidth="1"/>
+    <col min="6" max="6" width="23.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:6">
@@ -25769,34 +25775,34 @@
       <c r="D66" s="4"/>
       <c r="E66" s="4"/>
     </row>
-    <row r="71" spans="1:5" ht="15.5">
+    <row r="71" spans="1:5" ht="15.4">
       <c r="D71" s="3"/>
     </row>
-    <row r="72" spans="1:5" ht="15.5">
+    <row r="72" spans="1:5" ht="15.4">
       <c r="D72" s="3"/>
     </row>
-    <row r="73" spans="1:5" ht="15.5">
+    <row r="73" spans="1:5" ht="15.4">
       <c r="D73" s="3"/>
     </row>
-    <row r="74" spans="1:5" ht="15.5">
+    <row r="74" spans="1:5" ht="15.4">
       <c r="D74" s="3"/>
     </row>
-    <row r="75" spans="1:5" ht="15.5">
+    <row r="75" spans="1:5" ht="15.4">
       <c r="D75" s="3"/>
     </row>
-    <row r="76" spans="1:5" ht="15.5">
+    <row r="76" spans="1:5" ht="15.4">
       <c r="D76" s="3"/>
     </row>
-    <row r="77" spans="1:5" ht="15.5">
+    <row r="77" spans="1:5" ht="15.4">
       <c r="D77" s="3"/>
     </row>
-    <row r="78" spans="1:5" ht="15.5">
+    <row r="78" spans="1:5" ht="15.4">
       <c r="D78" s="3"/>
     </row>
-    <row r="79" spans="1:5" ht="15.5">
+    <row r="79" spans="1:5" ht="15.4">
       <c r="D79" s="3"/>
     </row>
-    <row r="80" spans="1:5" ht="15.5">
+    <row r="80" spans="1:5" ht="15.4">
       <c r="D80" s="3"/>
     </row>
   </sheetData>
@@ -25816,11 +25822,11 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.453125" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="7.46484375" defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="3" width="17.81640625" customWidth="1"/>
-    <col min="4" max="4" width="29.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="9" width="17.81640625" customWidth="1"/>
+    <col min="2" max="3" width="17.796875" customWidth="1"/>
+    <col min="4" max="4" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="9" width="17.796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:9">
@@ -25835,7 +25841,7 @@
       <c r="H4" s="20"/>
       <c r="I4" s="21"/>
     </row>
-    <row r="5" spans="2:9" ht="15" thickBot="1">
+    <row r="5" spans="2:9" ht="14.65" thickBot="1">
       <c r="B5" s="22" t="s">
         <v>12</v>
       </c>
@@ -26208,7 +26214,7 @@
       </c>
       <c r="I28" s="26"/>
     </row>
-    <row r="29" spans="2:10" ht="29">
+    <row r="29" spans="2:10" ht="28.5">
       <c r="B29" s="26"/>
       <c r="C29" s="33" t="s">
         <v>22</v>
@@ -26220,7 +26226,7 @@
       <c r="H29" s="33"/>
       <c r="I29" s="26"/>
     </row>
-    <row r="30" spans="2:10" ht="15" thickBot="1">
+    <row r="30" spans="2:10" ht="14.65" thickBot="1">
       <c r="B30" s="26"/>
       <c r="C30" s="34" t="s">
         <v>23</v>
@@ -26391,15 +26397,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8EF56F5-FFEC-4195-B835-F2DA1F364DE3}">
-  <dimension ref="B3:J11"/>
+  <dimension ref="B3:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25"/>
+  <cols>
+    <col min="10" max="10" width="9.06640625" style="11"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="2:10">
+    <row r="3" spans="2:11">
       <c r="B3" s="37" t="s">
         <v>35</v>
       </c>
@@ -26408,7 +26417,7 @@
       <c r="E3" s="38"/>
       <c r="F3" s="11"/>
     </row>
-    <row r="4" spans="2:10" ht="15" thickBot="1">
+    <row r="4" spans="2:11" ht="14.65" thickBot="1">
       <c r="B4" s="39" t="s">
         <v>12</v>
       </c>
@@ -26433,11 +26442,14 @@
       <c r="I4" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="J4" s="41" t="s">
+      <c r="J4" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="K4" s="41" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="2:10">
+    <row r="5" spans="2:11">
       <c r="D5">
         <v>1</v>
       </c>
@@ -26456,11 +26468,14 @@
       <c r="I5">
         <v>0</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="11">
+        <v>0</v>
+      </c>
+      <c r="K5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="2:10">
+    <row r="6" spans="2:11">
       <c r="D6">
         <v>1</v>
       </c>
@@ -26479,11 +26494,14 @@
       <c r="I6">
         <v>1</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" s="11">
+        <v>0</v>
+      </c>
+      <c r="K6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="2:10">
+    <row r="7" spans="2:11">
       <c r="D7">
         <v>1</v>
       </c>
@@ -26502,37 +26520,59 @@
       <c r="I7" s="11">
         <v>1</v>
       </c>
-      <c r="J7" s="11" t="s">
+      <c r="J7" s="11">
+        <v>0</v>
+      </c>
+      <c r="K7" s="11" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="2:10">
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="42"/>
+    <row r="8" spans="2:11">
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" s="11">
+        <v>0</v>
+      </c>
+      <c r="G8" s="11">
+        <v>0</v>
+      </c>
+      <c r="H8" s="11">
+        <v>0</v>
+      </c>
+      <c r="I8" s="11">
+        <v>0</v>
+      </c>
+      <c r="J8" s="11">
+        <v>1</v>
+      </c>
+      <c r="K8" s="42" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="9" spans="2:10">
+    <row r="9" spans="2:11">
       <c r="F9" s="11"/>
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
       <c r="I9" s="11"/>
-      <c r="J9" s="42"/>
+      <c r="K9" s="42"/>
     </row>
-    <row r="10" spans="2:10">
+    <row r="10" spans="2:11">
       <c r="F10" s="11"/>
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
       <c r="I10" s="11"/>
-      <c r="J10" s="42"/>
+      <c r="K10" s="42"/>
     </row>
-    <row r="11" spans="2:10">
+    <row r="11" spans="2:11">
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
       <c r="I11" s="11"/>
-      <c r="J11" s="42"/>
+      <c r="K11" s="42"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>